<commit_message>
Update data file: KIOSC_Finance_Data.xlsx
</commit_message>
<xml_diff>
--- a/data/KIOSC_Finance_Data.xlsx
+++ b/data/KIOSC_Finance_Data.xlsx
@@ -569,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="str">
-        <v>Invoiced</v>
+        <v>Paid</v>
       </c>
       <c r="J4" t="str">
         <v>Materials for outreach program</v>
@@ -578,7 +578,7 @@
         <v>2023-02-20</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>2025-04-24</v>
       </c>
       <c r="M4" t="str">
         <v>user</v>
@@ -772,7 +772,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -864,9 +864,67 @@
         <v>Created journal entry JE-20250424-003</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>AUDIT1745477662005</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="C4" t="str">
+        <v>7776af38-6226-4f6a-9d0e-68a9a692852f</v>
+      </c>
+      <c r="D4" t="str">
+        <v>UPDATE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>admin</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2025-04-24T06:54:22.005Z</v>
+      </c>
+      <c r="H4" t="str">
+        <v>{"before":{"id":"7776af38-6226-4f6a-9d0e-68a9a692852f","date":"2023-02-15","description":"Educational Materials","supplier":"f99c571b-2d0d-48a8-b6fa-ec0a2bc491c9","amount":"3450","paymentType":"1","paymentCenter":"2","program":"2","status":"Invoiced","notes":"Materials for outreach program","invoiceDate":"2023-02-20","paymentDate":"","createdBy":"user","createdAt":"2023-02-15T14:00:00.000Z"},"after":{"id":"7776af38-6226-4f6a-9d0e-68a9a692852f","date":"2023-02-15","description":"Educational Materials","supplier":"f99c571b-2d0d-48a8-b6fa-ec0a2bc491c9","amount":"3450","paymentType":"1","paymentCenter":"2","program":"2","status":"Paid","notes":"Materials for outreach program","invoiceDate":"2023-02-20","paymentDate":"2025-04-24","createdBy":"user","createdAt":"2023-02-15T14:00:00.000Z"}}</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Updated Expense 7776af38-6226-4f6a-9d0e-68a9a692852f</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>AUDIT1745477662005</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="C5" t="str">
+        <v>7776af38-6226-4f6a-9d0e-68a9a692852f</v>
+      </c>
+      <c r="D5" t="str">
+        <v>UPDATE</v>
+      </c>
+      <c r="E5" t="str">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>admin</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2025-04-24T06:54:22.005Z</v>
+      </c>
+      <c r="H5" t="str">
+        <v>{"before":{"id":"7776af38-6226-4f6a-9d0e-68a9a692852f","date":"2023-02-15","description":"Educational Materials","supplier":"f99c571b-2d0d-48a8-b6fa-ec0a2bc491c9","amount":"3450","paymentType":"1","paymentCenter":"2","program":"2","status":"Invoiced","notes":"Materials for outreach program","invoiceDate":"2023-02-20","paymentDate":"","createdBy":"user","createdAt":"2023-02-15T14:00:00.000Z"},"after":{"id":"7776af38-6226-4f6a-9d0e-68a9a692852f","date":"2023-02-15","description":"Educational Materials","supplier":"f99c571b-2d0d-48a8-b6fa-ec0a2bc491c9","amount":"3450","paymentType":"1","paymentCenter":"2","program":"2","status":"Paid","notes":"Materials for outreach program","invoiceDate":"2023-02-20","paymentDate":"2025-04-24","createdBy":"user","createdAt":"2023-02-15T14:00:00.000Z"}}</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Updated Expense 7776af38-6226-4f6a-9d0e-68a9a692852f</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>